<commit_message>
IDM evaluation formatting fix
</commit_message>
<xml_diff>
--- a/docs/evaluation/RuntimeNodeJS Performance Tests.xlsx
+++ b/docs/evaluation/RuntimeNodeJS Performance Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="540" windowWidth="18855" windowHeight="8130"/>
+    <workbookView xWindow="150" yWindow="540" windowWidth="18855" windowHeight="8130" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Average</t>
   </si>
@@ -58,6 +58,27 @@
   </si>
   <si>
     <t>Avg Time/Update</t>
+  </si>
+  <si>
+    <t>5 Data Object Reporters</t>
+  </si>
+  <si>
+    <t>10 Data Object Reporters</t>
+  </si>
+  <si>
+    <t>15 Data Object Reporters</t>
+  </si>
+  <si>
+    <t>20 Data Object Reporters</t>
+  </si>
+  <si>
+    <t>25 Data Object Reporters</t>
+  </si>
+  <si>
+    <t>30 Data Object Reporters</t>
+  </si>
+  <si>
+    <t>40 Data Object Reporters</t>
   </si>
 </sst>
 </file>
@@ -368,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -452,6 +473,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2157,6 +2179,768 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-PT"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Data Objects Synchronisation Performance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1st</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$38</c:f>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$38</c:f>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3rd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$F$38</c:f>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg Time/Update</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="128263296"/>
+        <c:axId val="128281984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="128263296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400"/>
+                  <a:t>Number  of Changes to Data Object</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400" baseline="0"/>
+                  <a:t> Reporter</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="128281984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="128281984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400"/>
+                  <a:t>Time to have all Observers</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400" baseline="0"/>
+                  <a:t> Synchronised with Reporter Changes (milliseconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="128263296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-PT"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2194,7 +2978,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>5 Data Object Reporters</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2311,7 +3095,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>10 Data Object Reporters</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2428,7 +3212,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>15 Data Object Reporters</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2545,7 +3329,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>20 Data Object Reporters</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2662,7 +3446,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>25 Data Object Reporters</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2779,7 +3563,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>30 Data Object Reporters</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2896,7 +3680,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>40 Data Object Reporters</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3267,6 +4051,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3275,13 +4089,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>66674</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -3592,7 +4406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="I10" workbookViewId="0">
       <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
@@ -4078,12 +4892,13 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="I5" sqref="I5:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="4" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" thickTop="1" thickBot="1">
@@ -4162,7 +4977,10 @@
       <c r="H4" s="21">
         <v>8.5</v>
       </c>
-      <c r="I4" s="12"/>
+      <c r="I4" s="12">
+        <f>1000/H4</f>
+        <v>117.64705882352941</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="16.5" thickBot="1">
       <c r="A5" s="17">
@@ -4189,7 +5007,10 @@
       <c r="H5" s="21">
         <v>7.7</v>
       </c>
-      <c r="I5" s="12"/>
+      <c r="I5" s="12">
+        <f t="shared" ref="I5:I38" si="0">1000/H5</f>
+        <v>129.87012987012986</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1">
       <c r="A6" s="17">
@@ -4216,7 +5037,10 @@
       <c r="H6" s="21">
         <v>5.8</v>
       </c>
-      <c r="I6" s="12"/>
+      <c r="I6" s="12">
+        <f t="shared" si="0"/>
+        <v>172.41379310344828</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="16.5" thickBot="1">
       <c r="A7" s="17">
@@ -4243,7 +5067,10 @@
       <c r="H7" s="21">
         <v>9.1999999999999993</v>
       </c>
-      <c r="I7" s="12"/>
+      <c r="I7" s="12">
+        <f t="shared" si="0"/>
+        <v>108.69565217391305</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="16.5" thickBot="1">
       <c r="A8" s="17">
@@ -4270,7 +5097,10 @@
       <c r="H8" s="21">
         <v>11</v>
       </c>
-      <c r="I8" s="12"/>
+      <c r="I8" s="12">
+        <f t="shared" si="0"/>
+        <v>90.909090909090907</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="16.5" thickBot="1">
       <c r="A9" s="17">
@@ -4297,7 +5127,10 @@
       <c r="H9" s="21">
         <v>6.8</v>
       </c>
-      <c r="I9" s="12"/>
+      <c r="I9" s="12">
+        <f t="shared" si="0"/>
+        <v>147.05882352941177</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1">
       <c r="A10" s="22">
@@ -4324,7 +5157,10 @@
       <c r="H10" s="16">
         <v>10.199999999999999</v>
       </c>
-      <c r="I10" s="12"/>
+      <c r="I10" s="12">
+        <f t="shared" si="0"/>
+        <v>98.039215686274517</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
       <c r="A11" s="17">
@@ -4351,7 +5187,10 @@
       <c r="H11" s="21">
         <v>5.7</v>
       </c>
-      <c r="I11" s="12"/>
+      <c r="I11" s="12">
+        <f t="shared" si="0"/>
+        <v>175.43859649122805</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1">
       <c r="A12" s="17">
@@ -4378,7 +5217,10 @@
       <c r="H12" s="21">
         <v>13</v>
       </c>
-      <c r="I12" s="12"/>
+      <c r="I12" s="12">
+        <f t="shared" si="0"/>
+        <v>76.92307692307692</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="16.5" thickBot="1">
       <c r="A13" s="17">
@@ -4405,7 +5247,10 @@
       <c r="H13" s="21">
         <v>8.6</v>
       </c>
-      <c r="I13" s="12"/>
+      <c r="I13" s="12">
+        <f t="shared" si="0"/>
+        <v>116.27906976744187</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="16.5" thickBot="1">
       <c r="A14" s="17">
@@ -4432,7 +5277,10 @@
       <c r="H14" s="21">
         <v>16.399999999999999</v>
       </c>
-      <c r="I14" s="12"/>
+      <c r="I14" s="12">
+        <f t="shared" si="0"/>
+        <v>60.975609756097569</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="16.5" thickBot="1">
       <c r="A15" s="17">
@@ -4459,7 +5307,10 @@
       <c r="H15" s="21">
         <v>10.1</v>
       </c>
-      <c r="I15" s="12"/>
+      <c r="I15" s="12">
+        <f t="shared" si="0"/>
+        <v>99.009900990099013</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="16.5" thickBot="1">
       <c r="A16" s="17">
@@ -4486,7 +5337,10 @@
       <c r="H16" s="21">
         <v>11.7</v>
       </c>
-      <c r="I16" s="12"/>
+      <c r="I16" s="12">
+        <f t="shared" si="0"/>
+        <v>85.470085470085479</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="16.5" thickBot="1">
       <c r="A17" s="22">
@@ -4513,7 +5367,10 @@
       <c r="H17" s="16">
         <v>6.4</v>
       </c>
-      <c r="I17" s="12"/>
+      <c r="I17" s="12">
+        <f t="shared" si="0"/>
+        <v>156.25</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
       <c r="A18" s="17">
@@ -4540,7 +5397,10 @@
       <c r="H18" s="21">
         <v>13</v>
       </c>
-      <c r="I18" s="12"/>
+      <c r="I18" s="12">
+        <f t="shared" si="0"/>
+        <v>76.92307692307692</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="16.5" thickBot="1">
       <c r="A19" s="17">
@@ -4567,7 +5427,10 @@
       <c r="H19" s="21">
         <v>7.4</v>
       </c>
-      <c r="I19" s="12"/>
+      <c r="I19" s="12">
+        <f t="shared" si="0"/>
+        <v>135.13513513513513</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="16.5" thickBot="1">
       <c r="A20" s="17">
@@ -4594,7 +5457,10 @@
       <c r="H20" s="21">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I20" s="12"/>
+      <c r="I20" s="12">
+        <f t="shared" si="0"/>
+        <v>196.07843137254903</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1">
       <c r="A21" s="17">
@@ -4621,7 +5487,10 @@
       <c r="H21" s="21">
         <v>17.899999999999999</v>
       </c>
-      <c r="I21" s="12"/>
+      <c r="I21" s="12">
+        <f t="shared" si="0"/>
+        <v>55.865921787709503</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="16.5" thickBot="1">
       <c r="A22" s="17">
@@ -4648,7 +5517,10 @@
       <c r="H22" s="21">
         <v>8.5</v>
       </c>
-      <c r="I22" s="12"/>
+      <c r="I22" s="12">
+        <f t="shared" si="0"/>
+        <v>117.64705882352941</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="16.5" thickBot="1">
       <c r="A23" s="17">
@@ -4675,7 +5547,10 @@
       <c r="H23" s="21">
         <v>10.6</v>
       </c>
-      <c r="I23" s="12"/>
+      <c r="I23" s="12">
+        <f t="shared" si="0"/>
+        <v>94.339622641509436</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="16.5" thickBot="1">
       <c r="A24" s="17">
@@ -4702,7 +5577,10 @@
       <c r="H24" s="21">
         <v>14.3</v>
       </c>
-      <c r="I24" s="12"/>
+      <c r="I24" s="12">
+        <f t="shared" si="0"/>
+        <v>69.930069930069934</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="16.5" thickBot="1">
       <c r="A25" s="17">
@@ -4729,7 +5607,10 @@
       <c r="H25" s="21">
         <v>7.7</v>
       </c>
-      <c r="I25" s="12"/>
+      <c r="I25" s="12">
+        <f t="shared" si="0"/>
+        <v>129.87012987012986</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="16.5" thickBot="1">
       <c r="A26" s="17">
@@ -4756,7 +5637,10 @@
       <c r="H26" s="21">
         <v>4.9000000000000004</v>
       </c>
-      <c r="I26" s="12"/>
+      <c r="I26" s="12">
+        <f t="shared" si="0"/>
+        <v>204.08163265306121</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="16.5" thickBot="1">
       <c r="A27" s="17">
@@ -4783,7 +5667,10 @@
       <c r="H27" s="21">
         <v>16.3</v>
       </c>
-      <c r="I27" s="12"/>
+      <c r="I27" s="12">
+        <f t="shared" si="0"/>
+        <v>61.349693251533736</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="16.5" thickBot="1">
       <c r="A28" s="17">
@@ -4810,7 +5697,10 @@
       <c r="H28" s="21">
         <v>7.6</v>
       </c>
-      <c r="I28" s="12"/>
+      <c r="I28" s="12">
+        <f t="shared" si="0"/>
+        <v>131.57894736842107</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="16.5" thickBot="1">
       <c r="A29" s="17">
@@ -4837,7 +5727,10 @@
       <c r="H29" s="21">
         <v>9.6</v>
       </c>
-      <c r="I29" s="12"/>
+      <c r="I29" s="12">
+        <f t="shared" si="0"/>
+        <v>104.16666666666667</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="16.5" thickBot="1">
       <c r="A30" s="17">
@@ -4864,7 +5757,10 @@
       <c r="H30" s="21">
         <v>6.6</v>
       </c>
-      <c r="I30" s="12"/>
+      <c r="I30" s="12">
+        <f t="shared" si="0"/>
+        <v>151.51515151515153</v>
+      </c>
     </row>
     <row r="31" spans="1:9" ht="16.5" thickBot="1">
       <c r="A31" s="17">
@@ -4891,7 +5787,10 @@
       <c r="H31" s="21">
         <v>11.2</v>
       </c>
-      <c r="I31" s="12"/>
+      <c r="I31" s="12">
+        <f t="shared" si="0"/>
+        <v>89.285714285714292</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="16.5" thickBot="1">
       <c r="A32" s="17">
@@ -4918,7 +5817,10 @@
       <c r="H32" s="21">
         <v>13</v>
       </c>
-      <c r="I32" s="12"/>
+      <c r="I32" s="12">
+        <f t="shared" si="0"/>
+        <v>76.92307692307692</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="16.5" thickBot="1">
       <c r="A33" s="17">
@@ -4945,7 +5847,10 @@
       <c r="H33" s="21">
         <v>8.5</v>
       </c>
-      <c r="I33" s="12"/>
+      <c r="I33" s="12">
+        <f t="shared" si="0"/>
+        <v>117.64705882352941</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="16.5" thickBot="1">
       <c r="A34" s="17">
@@ -4972,7 +5877,10 @@
       <c r="H34" s="21">
         <v>17.5</v>
       </c>
-      <c r="I34" s="12"/>
+      <c r="I34" s="12">
+        <f t="shared" si="0"/>
+        <v>57.142857142857146</v>
+      </c>
     </row>
     <row r="35" spans="1:9" ht="16.5" thickBot="1">
       <c r="A35" s="17">
@@ -4999,7 +5907,10 @@
       <c r="H35" s="21">
         <v>10.199999999999999</v>
       </c>
-      <c r="I35" s="12"/>
+      <c r="I35" s="12">
+        <f t="shared" si="0"/>
+        <v>98.039215686274517</v>
+      </c>
     </row>
     <row r="36" spans="1:9" ht="16.5" thickBot="1">
       <c r="A36" s="17">
@@ -5026,7 +5937,10 @@
       <c r="H36" s="21">
         <v>12.1</v>
       </c>
-      <c r="I36" s="12"/>
+      <c r="I36" s="12">
+        <f t="shared" si="0"/>
+        <v>82.644628099173559</v>
+      </c>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1">
       <c r="A37" s="17">
@@ -5053,7 +5967,10 @@
       <c r="H37" s="21">
         <v>16.2</v>
       </c>
-      <c r="I37" s="12"/>
+      <c r="I37" s="12">
+        <f t="shared" si="0"/>
+        <v>61.728395061728399</v>
+      </c>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1">
       <c r="A38" s="22">
@@ -5080,7 +5997,10 @@
       <c r="H38" s="16">
         <v>18</v>
       </c>
-      <c r="I38" s="12"/>
+      <c r="I38" s="12">
+        <f t="shared" si="0"/>
+        <v>55.555555555555557</v>
+      </c>
     </row>
     <row r="39" spans="1:9" ht="14.25" thickTop="1" thickBot="1">
       <c r="A39" s="12"/>
@@ -5110,8 +6030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="S49" sqref="S49"/>
+    <sheetView tabSelected="1" topLeftCell="F30" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5151,34 +6071,34 @@
         <v>13</v>
       </c>
       <c r="F3" s="12"/>
-      <c r="J3">
-        <v>5</v>
-      </c>
-      <c r="K3">
-        <v>10</v>
-      </c>
-      <c r="L3">
+      <c r="J3" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M3">
+      <c r="L3" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="N3">
-        <v>25</v>
-      </c>
-      <c r="O3">
-        <v>30</v>
-      </c>
-      <c r="P3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="17.25" thickTop="1" thickBot="1">
+    </row>
+    <row r="4" spans="1:16" ht="40.5" thickTop="1" thickBot="1">
       <c r="A4" s="17">
         <v>1</v>
       </c>
-      <c r="B4" s="18">
-        <v>5</v>
+      <c r="B4" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="18">
         <v>5</v>
@@ -5197,12 +6117,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.5" thickBot="1">
+    <row r="5" spans="1:16" ht="39.75" thickBot="1">
       <c r="A5" s="17">
         <v>2</v>
       </c>
-      <c r="B5" s="18">
-        <v>5</v>
+      <c r="B5" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="18">
         <v>10</v>

</xml_diff>